<commit_message>
Update Leave Card 5/10/2023 4:38 PM
</commit_message>
<xml_diff>
--- a/REGULAR/1-RETIRED/DEL MUNDO, ESTER.xlsx
+++ b/REGULAR/1-RETIRED/DEL MUNDO, ESTER.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE CARD\REGULAR\1-RETIRED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\REGULAR\1-RETIRED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C26E30-579E-4DC0-AED3-8A2C39D42118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7D0B5D-13A3-4E77-9DE1-ABCF75288133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
   </bookViews>
@@ -28,18 +28,10 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Sheet1!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Sheet1 (2)'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1329,10 +1321,10 @@
     <t>TOTAL VL = 27.831</t>
   </si>
   <si>
-    <t>OPTIONAL RETIREMENT EFFECTIVE DATE: DECEMBER 31, 2022</t>
-  </si>
-  <si>
     <t>ADMIN AIDE VI</t>
+  </si>
+  <si>
+    <t>OPTIONAL RETIREMENT EFFECTIVE DATE: JANUARY 01, 2023</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1338,7 @@
     <numFmt numFmtId="167" formatCode="dd"/>
     <numFmt numFmtId="168" formatCode="&quot;CM&quot;\-#######"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1402,6 +1394,19 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1591,7 +1596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1763,6 +1768,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1801,6 +1809,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4124,64 +4141,64 @@
       <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="59"/>
+      <c r="C2" s="60"/>
       <c r="D2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="9"/>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="63"/>
+      <c r="G2" s="64"/>
       <c r="H2" s="27" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="24"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
       <c r="D3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="60"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="61"/>
       <c r="H3" s="25" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="25"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="69"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="60"/>
+      <c r="G4" s="61"/>
       <c r="H4" s="25" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="25"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="62"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
@@ -4207,18 +4224,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62" t="s">
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -17533,9 +17550,9 @@
   <dimension ref="A2:M576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A567" activePane="bottomLeft"/>
-      <selection activeCell="M1" sqref="M1:M1048576"/>
-      <selection pane="bottomLeft" activeCell="F570" sqref="F570"/>
+      <pane ySplit="3576" topLeftCell="A560" activePane="bottomLeft"/>
+      <selection activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="E564" sqref="E564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17557,68 +17574,68 @@
       <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="59"/>
+      <c r="C2" s="60"/>
       <c r="D2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="9"/>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="63"/>
+      <c r="G2" s="64"/>
       <c r="H2" s="27" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="24"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="59" t="s">
-        <v>428</v>
-      </c>
-      <c r="C3" s="59"/>
+      <c r="B3" s="60" t="s">
+        <v>427</v>
+      </c>
+      <c r="C3" s="60"/>
       <c r="D3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="66">
+      <c r="F3" s="67">
         <v>29845</v>
       </c>
-      <c r="G3" s="60"/>
+      <c r="G3" s="61"/>
       <c r="H3" s="25" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="25"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="69"/>
     </row>
     <row r="4" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="60"/>
+      <c r="G4" s="61"/>
       <c r="H4" s="25" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="25"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="62"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
@@ -17644,18 +17661,18 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62" t="s">
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -17701,8 +17718,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="10"/>
       <c r="E9" s="12">
-        <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>27.83100000000012</v>
+        <v>31.913</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="12" t="str">
@@ -17711,8 +17727,7 @@
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="12">
-        <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>81.222000000000051</v>
+        <v>61.805999999999997</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="19"/>
@@ -17722,7 +17737,7 @@
       <c r="A10" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="12"/>
       <c r="D10" s="36"/>
       <c r="E10" s="33"/>
@@ -30389,7 +30404,7 @@
     <row r="573" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A573" s="56"/>
       <c r="B573" s="57" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C573" s="52"/>
       <c r="D573" s="53"/>
@@ -30405,13 +30420,13 @@
       <c r="A574" s="37"/>
       <c r="B574" s="19"/>
       <c r="C574" s="12"/>
-      <c r="D574" s="58" t="s">
+      <c r="D574" s="73" t="s">
         <v>426</v>
       </c>
-      <c r="E574" s="8"/>
-      <c r="F574" s="19"/>
-      <c r="G574" s="8"/>
-      <c r="H574" s="58" t="s">
+      <c r="E574" s="74"/>
+      <c r="F574" s="75"/>
+      <c r="G574" s="74"/>
+      <c r="H574" s="73" t="s">
         <v>424</v>
       </c>
       <c r="I574" s="8"/>
@@ -30466,7 +30481,7 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{3C67B38A-DE91-4BA1-85D0-F5C61D6395E6}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
@@ -30482,7 +30497,7 @@
 EMPLOYEE'S LEAVE CARD</oddHeader>
     <oddFooter>&amp;L
 PREPARED BY: &amp;UJUEL D. COPER&amp;U
-DATE: &amp;D, &amp;T&amp;C
+DATE: 12/14/2022, 12:36 PM&amp;C
 CERTIFIED CORRECT BY: &amp;UALMA A. MALABANAN&amp;U
                                    HRMO&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -30516,17 +30531,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="J1" s="70" t="s">
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="J1" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
@@ -30611,12 +30626,12 @@
         <v>30</v>
       </c>
       <c r="G6" s="42"/>
-      <c r="I6" s="71" t="s">
+      <c r="I6" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="44">

</xml_diff>